<commit_message>
Update email templates and styles for complaint management; add Net Promoter Score and improve design consistency
</commit_message>
<xml_diff>
--- a/Fullr Burgers/EH (Fullr).xlsx
+++ b/Fullr Burgers/EH (Fullr).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSM Projects\Fullr Burgers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B56ABE7-1A9A-4327-A53B-A7591DA737C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2C56E8-284A-4616-9223-1ED85159CAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Location</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Crescat</t>
   </si>
   <si>
-    <t>Colombo 05</t>
-  </si>
-  <si>
     <t>Mount Lavinia</t>
   </si>
   <si>
@@ -50,14 +47,31 @@
   </si>
   <si>
     <t>Colombo City Centre (CCC)</t>
+  </si>
+  <si>
+    <t>Port City Colombo</t>
+  </si>
+  <si>
+    <t>Negombo</t>
+  </si>
+  <si>
+    <t>Thalahena</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,58 +441,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -487,10 +502,21 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:A9" numberStoredAsText="1"/>
+    <ignoredError sqref="A2 A3:A8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>